<commit_message>
added ui features and major backend connection
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbpat\myWebsites\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8209AE82-2559-4CDA-86E3-ADA26E6A3F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3148868-8223-43BA-A922-F380B5FEF784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{28665C28-DE42-4A0F-911C-3133FEF14900}"/>
   </bookViews>
@@ -25,72 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
   <si>
-    <t>sfjsfdjsf</t>
+    <t>HTML stands for -</t>
   </si>
   <si>
-    <t>jkjhkjh</t>
+    <t>HighText Machine Language</t>
   </si>
   <si>
-    <t>klkk</t>
+    <t>HyperText and links Markup Language</t>
   </si>
   <si>
-    <t>kjbkkj</t>
+    <t>HyperText Markup Language</t>
   </si>
   <si>
-    <t>kjkjhkjh</t>
-  </si>
-  <si>
-    <t>kjkj</t>
-  </si>
-  <si>
-    <t>ljhjhkjh</t>
-  </si>
-  <si>
-    <t>kjh;ljh</t>
-  </si>
-  <si>
-    <t>kkjh</t>
-  </si>
-  <si>
-    <t>kbljh</t>
-  </si>
-  <si>
-    <t>sfkjsekj</t>
-  </si>
-  <si>
-    <t>lkjkjkjpj</t>
-  </si>
-  <si>
-    <t>jpopj</t>
-  </si>
-  <si>
-    <t>kjkjbkjb</t>
-  </si>
-  <si>
-    <t>ljnjn</t>
-  </si>
-  <si>
-    <t>jnljn</t>
-  </si>
-  <si>
-    <t>jhguuoh</t>
-  </si>
-  <si>
-    <t>kjhijhoho</t>
-  </si>
-  <si>
-    <t>kjhohoho</t>
-  </si>
-  <si>
-    <t>hooo</t>
-  </si>
-  <si>
-    <t>hohuiu</t>
-  </si>
-  <si>
-    <t>kbk</t>
+    <t>None of these</t>
   </si>
 </sst>
 </file>
@@ -442,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EDF064B-C436-4D8A-994D-5A4A991D0040}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,82 +404,103 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>